<commit_message>
Working Excel, Json not yet
</commit_message>
<xml_diff>
--- a/examples/VehiclesDatabase.xlsx
+++ b/examples/VehiclesDatabase.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoprisan/Desktop/Java-Dev-Bootcamp-2018/IdeaPlayGround/FirstProgram/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE39097-17E6-0C42-A416-86890C723AFC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="5840" windowWidth="27640" windowHeight="16940" xr2:uid="{E765D13C-9091-714E-A4F4-2BE31E9CD727}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -407,21 +406,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20A28CF-A4C2-284D-9B75-26ECCC45DD60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -441,7 +440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -461,7 +460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -481,7 +480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>